<commit_message>
construcción de lógica de selección de pairings y perfil de sabor
</commit_message>
<xml_diff>
--- a/src/data/raw/meals/Meals.xlsx
+++ b/src/data/raw/meals/Meals.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Usuario\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B160B8AD-A4D6-4194-B1BF-E29D0A257A7C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C26832FE-309B-479E-B501-5E5C926DB10D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{815E471D-FB27-4CE8-A9B5-FEF30EA8CD57}"/>
   </bookViews>
@@ -62,9 +62,6 @@
     <t>cured meat</t>
   </si>
   <si>
-    <t>game (deer venison)</t>
-  </si>
-  <si>
     <t>goat's milk cheese</t>
   </si>
   <si>
@@ -92,9 +89,6 @@
     <t>poultry</t>
   </si>
   <si>
-    <t>rich fish (salmon tuna etc)</t>
-  </si>
-  <si>
     <t>shellfish</t>
   </si>
   <si>
@@ -113,9 +107,6 @@
     <t>Salmón a la Plancha</t>
   </si>
   <si>
-    <t>Rich Fish (salmon tuna etc)</t>
-  </si>
-  <si>
     <t>Poultry</t>
   </si>
   <si>
@@ -158,9 +149,6 @@
     <t>Ciervo Estofado</t>
   </si>
   <si>
-    <t>Game (deer venison)</t>
-  </si>
-  <si>
     <t>Lean Fish</t>
   </si>
   <si>
@@ -312,6 +300,18 @@
   </si>
   <si>
     <t>Tortilla de Papa</t>
+  </si>
+  <si>
+    <t>game (deer, venison)</t>
+  </si>
+  <si>
+    <t>rich fish (salmon, tuna, etc)</t>
+  </si>
+  <si>
+    <t>Game (deer, venison)</t>
+  </si>
+  <si>
+    <t>Rich Fish (salmon, tuna, etc)</t>
   </si>
 </sst>
 </file>
@@ -685,11 +685,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{788D91E9-4975-43F6-A96D-CD05AC054CF1}">
   <dimension ref="A1:V53"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C23" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight"/>
+      <selection pane="bottomRight" activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -721,57 +721,57 @@
         <v>6</v>
       </c>
       <c r="H1" t="s">
+        <v>87</v>
+      </c>
+      <c r="I1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>11</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>12</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>13</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>14</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q1" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="R1" t="s">
+        <v>88</v>
+      </c>
+      <c r="S1" t="s">
         <v>16</v>
       </c>
-      <c r="R1" t="s">
+      <c r="T1" t="s">
         <v>17</v>
       </c>
-      <c r="S1" t="s">
+      <c r="U1" t="s">
         <v>18</v>
       </c>
-      <c r="T1" t="s">
+      <c r="V1" t="s">
         <v>19</v>
-      </c>
-      <c r="U1" t="s">
-        <v>20</v>
-      </c>
-      <c r="V1" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="2" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="B2" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="C2">
         <v>0</v>
@@ -836,10 +836,10 @@
     </row>
     <row r="3" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="B3" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="C3">
         <v>0</v>
@@ -904,10 +904,10 @@
     </row>
     <row r="4" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="B4" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="C4">
         <v>1</v>
@@ -972,10 +972,10 @@
     </row>
     <row r="5" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="B5" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="C5">
         <v>0</v>
@@ -1040,10 +1040,10 @@
     </row>
     <row r="6" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="B6" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="C6">
         <v>0</v>
@@ -1108,10 +1108,10 @@
     </row>
     <row r="7" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="B7" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="C7">
         <v>0</v>
@@ -1176,10 +1176,10 @@
     </row>
     <row r="8" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="B8" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="C8">
         <v>0</v>
@@ -1244,10 +1244,10 @@
     </row>
     <row r="9" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="B9" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="C9">
         <v>0</v>
@@ -1312,10 +1312,10 @@
     </row>
     <row r="10" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="B10" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="C10">
         <v>0</v>
@@ -1380,10 +1380,10 @@
     </row>
     <row r="11" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="B11" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="C11">
         <v>0</v>
@@ -1448,10 +1448,10 @@
     </row>
     <row r="12" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="B12" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="C12">
         <v>0</v>
@@ -1516,10 +1516,10 @@
     </row>
     <row r="13" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="B13" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="C13">
         <v>0</v>
@@ -1584,10 +1584,10 @@
     </row>
     <row r="14" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="B14" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="C14">
         <v>0</v>
@@ -1652,10 +1652,10 @@
     </row>
     <row r="15" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="B15" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="C15">
         <v>0</v>
@@ -1720,10 +1720,10 @@
     </row>
     <row r="16" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="B16" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="C16">
         <v>0</v>
@@ -1788,10 +1788,10 @@
     </row>
     <row r="17" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="B17" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="C17">
         <v>0</v>
@@ -1856,10 +1856,10 @@
     </row>
     <row r="18" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B18" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="C18">
         <v>1</v>
@@ -1924,10 +1924,10 @@
     </row>
     <row r="19" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="B19" t="s">
-        <v>39</v>
+        <v>89</v>
       </c>
       <c r="C19">
         <v>0</v>
@@ -1992,10 +1992,10 @@
     </row>
     <row r="20" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="B20" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="C20">
         <v>0</v>
@@ -2060,10 +2060,10 @@
     </row>
     <row r="21" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="B21" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="C21">
         <v>0</v>
@@ -2128,10 +2128,10 @@
     </row>
     <row r="22" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="B22" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="C22">
         <v>0</v>
@@ -2196,10 +2196,10 @@
     </row>
     <row r="23" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="B23" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="C23">
         <v>0</v>
@@ -2264,10 +2264,10 @@
     </row>
     <row r="24" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="B24" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="C24">
         <v>0</v>
@@ -2332,10 +2332,10 @@
     </row>
     <row r="25" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="B25" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C25">
         <v>0</v>
@@ -2400,10 +2400,10 @@
     </row>
     <row r="26" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="B26" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C26">
         <v>0</v>
@@ -2468,10 +2468,10 @@
     </row>
     <row r="27" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="B27" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C27">
         <v>0</v>
@@ -2536,10 +2536,10 @@
     </row>
     <row r="28" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="B28" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C28">
         <v>0</v>
@@ -2604,10 +2604,10 @@
     </row>
     <row r="29" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="B29" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="C29">
         <v>0</v>
@@ -2672,10 +2672,10 @@
     </row>
     <row r="30" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="B30" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="C30">
         <v>0</v>
@@ -2740,10 +2740,10 @@
     </row>
     <row r="31" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="B31" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="C31">
         <v>0</v>
@@ -2808,10 +2808,10 @@
     </row>
     <row r="32" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="B32" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="C32">
         <v>0</v>
@@ -2876,10 +2876,10 @@
     </row>
     <row r="33" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="B33" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="C33">
         <v>0</v>
@@ -2944,10 +2944,10 @@
     </row>
     <row r="34" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="B34" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C34">
         <v>0</v>
@@ -3012,10 +3012,10 @@
     </row>
     <row r="35" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="B35" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C35">
         <v>0</v>
@@ -3080,10 +3080,10 @@
     </row>
     <row r="36" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="B36" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C36">
         <v>0</v>
@@ -3148,10 +3148,10 @@
     </row>
     <row r="37" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="B37" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C37">
         <v>0</v>
@@ -3216,10 +3216,10 @@
     </row>
     <row r="38" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="B38" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C38">
         <v>0</v>
@@ -3284,10 +3284,10 @@
     </row>
     <row r="39" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B39" t="s">
-        <v>24</v>
+        <v>90</v>
       </c>
       <c r="C39">
         <v>0</v>
@@ -3352,10 +3352,10 @@
     </row>
     <row r="40" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="B40" t="s">
-        <v>24</v>
+        <v>90</v>
       </c>
       <c r="C40">
         <v>0</v>
@@ -3420,10 +3420,10 @@
     </row>
     <row r="41" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="B41" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="C41">
         <v>0</v>
@@ -3488,10 +3488,10 @@
     </row>
     <row r="42" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="B42" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="C42">
         <v>0</v>
@@ -3556,10 +3556,10 @@
     </row>
     <row r="43" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="B43" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="C43">
         <v>1</v>
@@ -3624,10 +3624,10 @@
     </row>
     <row r="44" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="B44" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="C44">
         <v>0</v>
@@ -3692,10 +3692,10 @@
     </row>
     <row r="45" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="B45" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="C45">
         <v>0</v>
@@ -3760,10 +3760,10 @@
     </row>
     <row r="46" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="B46" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="C46">
         <v>0</v>
@@ -3828,10 +3828,10 @@
     </row>
     <row r="47" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="B47" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="C47">
         <v>0</v>
@@ -3896,10 +3896,10 @@
     </row>
     <row r="48" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="B48" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="C48">
         <v>0</v>
@@ -3964,10 +3964,10 @@
     </row>
     <row r="49" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="B49" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="C49">
         <v>0</v>
@@ -4032,10 +4032,10 @@
     </row>
     <row r="50" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="B50" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="C50">
         <v>0</v>
@@ -4100,10 +4100,10 @@
     </row>
     <row r="51" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="B51" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="C51">
         <v>0</v>
@@ -4168,10 +4168,10 @@
     </row>
     <row r="52" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="B52" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="C52">
         <v>0</v>
@@ -4236,10 +4236,10 @@
     </row>
     <row r="53" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="B53" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="C53">
         <v>0</v>
@@ -4303,11 +4303,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:V37" xr:uid="{788D91E9-4975-43F6-A96D-CD05AC054CF1}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:V52">
-      <sortCondition ref="B1:B37"/>
-    </sortState>
-  </autoFilter>
+  <autoFilter ref="A1:V37" xr:uid="{788D91E9-4975-43F6-A96D-CD05AC054CF1}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Small fixes synthetic user
</commit_message>
<xml_diff>
--- a/src/data/raw/meals/Meals.xlsx
+++ b/src/data/raw/meals/Meals.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Usuario\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C26832FE-309B-479E-B501-5E5C926DB10D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF44A92B-F229-4038-B9E4-CBC4D487B74B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{815E471D-FB27-4CE8-A9B5-FEF30EA8CD57}"/>
   </bookViews>
@@ -311,7 +311,7 @@
     <t>Game (deer, venison)</t>
   </si>
   <si>
-    <t>Rich Fish (salmon, tuna, etc)</t>
+    <t>Rich Fish (salmon, tuna etc)</t>
   </si>
 </sst>
 </file>
@@ -686,10 +686,10 @@
   <dimension ref="A1:V53"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C20" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E6" sqref="E6"/>
+      <selection pane="bottomRight" activeCell="B40" sqref="B40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>